<commit_message>
update TOGS lof files
</commit_message>
<xml_diff>
--- a/figureinfo/TOGS-lof5.xlsx
+++ b/figureinfo/TOGS-lof5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\friendly\Dropbox\DVH Website Templating Code\figureinfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\Rprojects\HistDataVis\figureinfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80FCB19-01B4-4CAF-ADB7-9138452B8344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9994EC-D68B-45D1-9436-B65E37AD1198}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="1410" windowWidth="23940" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="285" yWindow="585" windowWidth="24285" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1210,9 +1210,6 @@
     <t xml:space="preserve">Classified by place of development. Tick marks at the bottom show individual events. The smoothed curves plot their relative frequency, in Europe and North America. </t>
   </si>
   <si>
-    <t>(a) A clay cuneiform tablet dated as 3300–3100 BCE, giving an account of yields of barley; (b) quipus, a system of knots tied in ropes used by South American Incas, around 1000 CE; (c) symbols used in Mayan culture, around 500 CE, showing the numbers 0–19; (d) a scheme proposed by John W. Tukey (1977) to tally counts of observations by hand, using dots and lines in groups of 10. Sources: (a) Britannica.com; (b) L. Leland Locke, The Ancient Quipu, Washington, DC: The American Museum of Natural History, 1923, fig. 1; (c) Neuromancer2K4 / Bryan Derksen / Wikimedia Commons / GNU Free Documentation License; (d) Pinethicket / Wikimedia Commons / GNU Free Documentation License.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Successive moments of a wrestling match between two people. From a drawing on the east wall of the tomb of Baqt at the Beni Hasan cemetery (ca. 2000 BCE). </t>
   </si>
   <si>
@@ -1894,7 +1891,10 @@
     <t>09_14-randu-combined.png</t>
   </si>
   <si>
-    <t>Various sources</t>
+    <t>(a) A clay cuneiform tablet dated as 3300–3100 BCE, giving an account of yields of barley; (b) quipus, a system of knots tied in ropes used by South American Incas, around 1000 CE; (c) symbols used in Mayan culture, around 500 CE, showing the numbers 0–19; (d) a scheme proposed by John W. Tukey (1977) to tally counts of observations by hand, using dots and lines in groups of 10.  Wikimedia Commons / GNU Free Documentation License.</t>
+  </si>
+  <si>
+    <t>Sources: (a) Britannica.com; (b) L. Leland Locke, The Ancient Quipu, Washington, DC: The American Museum of Natural History, 1923, fig. 1; (c) Neuromancer2K4 / Bryan Derksen / Wikimedia Commons / GNU Free Documentation License; (d) Pinethicket /</t>
   </si>
 </sst>
 </file>
@@ -2249,8 +2249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84:A112"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2303,7 +2303,7 @@
         <v>395</v>
       </c>
       <c r="G2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2323,7 +2323,7 @@
         <v>267</v>
       </c>
       <c r="F3" t="s">
-        <v>396</v>
+        <v>623</v>
       </c>
       <c r="G3" t="s">
         <v>624</v>
@@ -2346,10 +2346,10 @@
         <v>268</v>
       </c>
       <c r="F4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2369,10 +2369,10 @@
         <v>269</v>
       </c>
       <c r="F5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2392,10 +2392,10 @@
         <v>270</v>
       </c>
       <c r="F6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G6" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2415,10 +2415,10 @@
         <v>271</v>
       </c>
       <c r="F7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2438,10 +2438,10 @@
         <v>272</v>
       </c>
       <c r="F8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G8" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2461,10 +2461,10 @@
         <v>273</v>
       </c>
       <c r="F9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G9" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2484,10 +2484,10 @@
         <v>274</v>
       </c>
       <c r="F10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G10" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2507,10 +2507,10 @@
         <v>275</v>
       </c>
       <c r="F11" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G11" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2530,10 +2530,10 @@
         <v>276</v>
       </c>
       <c r="F12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G12" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2553,10 +2553,10 @@
         <v>277</v>
       </c>
       <c r="F13" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2576,10 +2576,10 @@
         <v>278</v>
       </c>
       <c r="F14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G14" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2599,10 +2599,10 @@
         <v>279</v>
       </c>
       <c r="F15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G15" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2622,10 +2622,10 @@
         <v>280</v>
       </c>
       <c r="F16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G16" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2645,10 +2645,10 @@
         <v>281</v>
       </c>
       <c r="F17" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2668,10 +2668,10 @@
         <v>282</v>
       </c>
       <c r="F18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G18" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2691,10 +2691,10 @@
         <v>283</v>
       </c>
       <c r="F19" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G19" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2714,10 +2714,10 @@
         <v>284</v>
       </c>
       <c r="F20" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G20" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2737,10 +2737,10 @@
         <v>285</v>
       </c>
       <c r="F21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G21" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2760,10 +2760,10 @@
         <v>286</v>
       </c>
       <c r="F22" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G22" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2783,10 +2783,10 @@
         <v>287</v>
       </c>
       <c r="F23" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G23" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2806,10 +2806,10 @@
         <v>288</v>
       </c>
       <c r="F24" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G24" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2829,10 +2829,10 @@
         <v>289</v>
       </c>
       <c r="F25" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G25" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2852,10 +2852,10 @@
         <v>290</v>
       </c>
       <c r="F26" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G26" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2875,10 +2875,10 @@
         <v>291</v>
       </c>
       <c r="F27" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G27" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2898,10 +2898,10 @@
         <v>292</v>
       </c>
       <c r="F28" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G28" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2921,10 +2921,10 @@
         <v>293</v>
       </c>
       <c r="F29" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G29" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2944,10 +2944,10 @@
         <v>294</v>
       </c>
       <c r="F30" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G30" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2967,10 +2967,10 @@
         <v>295</v>
       </c>
       <c r="F31" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G31" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2990,10 +2990,10 @@
         <v>296</v>
       </c>
       <c r="F32" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G32" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -3013,10 +3013,10 @@
         <v>297</v>
       </c>
       <c r="F33" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G33" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -3036,10 +3036,10 @@
         <v>298</v>
       </c>
       <c r="F34" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G34" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -3059,10 +3059,10 @@
         <v>299</v>
       </c>
       <c r="F35" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G35" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -3082,10 +3082,10 @@
         <v>300</v>
       </c>
       <c r="F36" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G36" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -3105,10 +3105,10 @@
         <v>301</v>
       </c>
       <c r="F37" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G37" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3128,10 +3128,10 @@
         <v>302</v>
       </c>
       <c r="F38" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G38" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3151,10 +3151,10 @@
         <v>303</v>
       </c>
       <c r="F39" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G39" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3174,10 +3174,10 @@
         <v>304</v>
       </c>
       <c r="F40" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G40" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -3197,10 +3197,10 @@
         <v>305</v>
       </c>
       <c r="F41" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G41" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3220,10 +3220,10 @@
         <v>306</v>
       </c>
       <c r="F42" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G42" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -3243,10 +3243,10 @@
         <v>307</v>
       </c>
       <c r="F43" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G43" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3266,10 +3266,10 @@
         <v>308</v>
       </c>
       <c r="F44" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G44" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -3289,10 +3289,10 @@
         <v>309</v>
       </c>
       <c r="F45" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G45" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3312,10 +3312,10 @@
         <v>310</v>
       </c>
       <c r="F46" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G46" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -3335,10 +3335,10 @@
         <v>311</v>
       </c>
       <c r="F47" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G47" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -3358,10 +3358,10 @@
         <v>312</v>
       </c>
       <c r="F48" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G48" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3381,10 +3381,10 @@
         <v>313</v>
       </c>
       <c r="F49" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G49" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -3404,10 +3404,10 @@
         <v>314</v>
       </c>
       <c r="F50" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G50" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -3427,10 +3427,10 @@
         <v>315</v>
       </c>
       <c r="F51" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G51" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3450,10 +3450,10 @@
         <v>316</v>
       </c>
       <c r="F52" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G52" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3473,10 +3473,10 @@
         <v>317</v>
       </c>
       <c r="F53" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G53" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -3496,10 +3496,10 @@
         <v>318</v>
       </c>
       <c r="F54" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G54" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -3519,10 +3519,10 @@
         <v>319</v>
       </c>
       <c r="F55" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G55" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -3542,10 +3542,10 @@
         <v>320</v>
       </c>
       <c r="F56" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G56" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3565,10 +3565,10 @@
         <v>321</v>
       </c>
       <c r="F57" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G57" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -3588,10 +3588,10 @@
         <v>322</v>
       </c>
       <c r="F58" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G58" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3611,10 +3611,10 @@
         <v>323</v>
       </c>
       <c r="F59" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G59" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -3634,10 +3634,10 @@
         <v>324</v>
       </c>
       <c r="F60" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G60" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -3657,10 +3657,10 @@
         <v>325</v>
       </c>
       <c r="F61" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G61" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3680,10 +3680,10 @@
         <v>326</v>
       </c>
       <c r="F62" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G62" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3703,10 +3703,10 @@
         <v>327</v>
       </c>
       <c r="F63" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G63" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3726,10 +3726,10 @@
         <v>328</v>
       </c>
       <c r="F64" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G64" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3749,10 +3749,10 @@
         <v>329</v>
       </c>
       <c r="F65" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G65" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3772,10 +3772,10 @@
         <v>330</v>
       </c>
       <c r="F66" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G66" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3789,16 +3789,16 @@
         <v>72</v>
       </c>
       <c r="D67" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E67" t="s">
         <v>331</v>
       </c>
       <c r="F67" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G67" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3818,10 +3818,10 @@
         <v>332</v>
       </c>
       <c r="F68" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G68" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3841,10 +3841,10 @@
         <v>333</v>
       </c>
       <c r="F69" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G69" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3864,10 +3864,10 @@
         <v>334</v>
       </c>
       <c r="F70" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G70" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -3887,10 +3887,10 @@
         <v>335</v>
       </c>
       <c r="F71" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G71" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3910,10 +3910,10 @@
         <v>336</v>
       </c>
       <c r="F72" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G72" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3933,10 +3933,10 @@
         <v>337</v>
       </c>
       <c r="F73" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G73" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3956,10 +3956,10 @@
         <v>338</v>
       </c>
       <c r="F74" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G74" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3979,10 +3979,10 @@
         <v>339</v>
       </c>
       <c r="F75" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G75" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -4002,10 +4002,10 @@
         <v>340</v>
       </c>
       <c r="F76" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G76" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -4025,10 +4025,10 @@
         <v>341</v>
       </c>
       <c r="F77" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G77" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -4048,10 +4048,10 @@
         <v>342</v>
       </c>
       <c r="F78" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G78" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -4071,10 +4071,10 @@
         <v>343</v>
       </c>
       <c r="F79" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G79" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -4094,10 +4094,10 @@
         <v>344</v>
       </c>
       <c r="F80" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G80" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -4117,10 +4117,10 @@
         <v>345</v>
       </c>
       <c r="F81" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G81" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -4140,10 +4140,10 @@
         <v>346</v>
       </c>
       <c r="F82" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G82" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -4163,10 +4163,10 @@
         <v>347</v>
       </c>
       <c r="F83" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G83" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -4186,10 +4186,10 @@
         <v>348</v>
       </c>
       <c r="F84" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G84" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4209,10 +4209,10 @@
         <v>349</v>
       </c>
       <c r="F85" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G85" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4232,10 +4232,10 @@
         <v>350</v>
       </c>
       <c r="F86" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G86" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -4255,10 +4255,10 @@
         <v>351</v>
       </c>
       <c r="F87" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G87" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -4278,10 +4278,10 @@
         <v>352</v>
       </c>
       <c r="F88" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G88" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -4301,10 +4301,10 @@
         <v>353</v>
       </c>
       <c r="F89" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G89" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -4324,10 +4324,10 @@
         <v>354</v>
       </c>
       <c r="F90" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G90" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -4347,10 +4347,10 @@
         <v>355</v>
       </c>
       <c r="F91" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G91" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -4370,10 +4370,10 @@
         <v>356</v>
       </c>
       <c r="F92" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G92" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -4393,10 +4393,10 @@
         <v>357</v>
       </c>
       <c r="F93" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G93" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -4416,10 +4416,10 @@
         <v>358</v>
       </c>
       <c r="F94" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G94" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -4439,10 +4439,10 @@
         <v>359</v>
       </c>
       <c r="F95" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G95" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -4462,10 +4462,10 @@
         <v>360</v>
       </c>
       <c r="F96" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G96" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -4485,10 +4485,10 @@
         <v>361</v>
       </c>
       <c r="F97" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G97" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -4502,16 +4502,16 @@
         <v>103</v>
       </c>
       <c r="D98" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E98" t="s">
         <v>362</v>
       </c>
       <c r="F98" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G98" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -4531,10 +4531,10 @@
         <v>363</v>
       </c>
       <c r="F99" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G99" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -4554,10 +4554,10 @@
         <v>364</v>
       </c>
       <c r="F100" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G100" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -4577,10 +4577,10 @@
         <v>365</v>
       </c>
       <c r="F101" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G101" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -4600,10 +4600,10 @@
         <v>366</v>
       </c>
       <c r="F102" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G102" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -4623,10 +4623,10 @@
         <v>367</v>
       </c>
       <c r="F103" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G103" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -4646,10 +4646,10 @@
         <v>368</v>
       </c>
       <c r="F104" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="G104" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -4669,10 +4669,10 @@
         <v>369</v>
       </c>
       <c r="F105" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G105" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -4692,10 +4692,10 @@
         <v>370</v>
       </c>
       <c r="F106" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G106" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -4715,10 +4715,10 @@
         <v>371</v>
       </c>
       <c r="F107" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G107" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -4738,10 +4738,10 @@
         <v>372</v>
       </c>
       <c r="F108" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G108" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -4761,10 +4761,10 @@
         <v>373</v>
       </c>
       <c r="F109" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G109" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -4784,10 +4784,10 @@
         <v>374</v>
       </c>
       <c r="F110" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G110" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -4807,10 +4807,10 @@
         <v>374</v>
       </c>
       <c r="F111" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G111" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -4830,10 +4830,10 @@
         <v>375</v>
       </c>
       <c r="F112" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G112" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -4853,10 +4853,10 @@
         <v>376</v>
       </c>
       <c r="F113" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G113" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -4876,10 +4876,10 @@
         <v>377</v>
       </c>
       <c r="F114" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G114" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -4899,10 +4899,10 @@
         <v>378</v>
       </c>
       <c r="F115" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G115" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -4922,10 +4922,10 @@
         <v>379</v>
       </c>
       <c r="F116" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G116" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -4945,10 +4945,10 @@
         <v>380</v>
       </c>
       <c r="F117" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G117" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -4968,10 +4968,10 @@
         <v>381</v>
       </c>
       <c r="F118" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G118" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -4991,15 +4991,15 @@
         <v>382</v>
       </c>
       <c r="F119" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G119" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B120">
         <v>8</v>
@@ -5014,10 +5014,10 @@
         <v>383</v>
       </c>
       <c r="F120" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G120" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -5037,10 +5037,10 @@
         <v>384</v>
       </c>
       <c r="F121" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G121" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -5060,10 +5060,10 @@
         <v>385</v>
       </c>
       <c r="F122" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G122" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -5083,10 +5083,10 @@
         <v>386</v>
       </c>
       <c r="F123" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G123" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -5106,10 +5106,10 @@
         <v>387</v>
       </c>
       <c r="F124" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G124" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -5129,10 +5129,10 @@
         <v>387</v>
       </c>
       <c r="F125" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G125" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -5152,10 +5152,10 @@
         <v>388</v>
       </c>
       <c r="F126" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G126" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -5175,10 +5175,10 @@
         <v>389</v>
       </c>
       <c r="F127" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G127" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -5198,10 +5198,10 @@
         <v>390</v>
       </c>
       <c r="F128" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G128" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -5215,16 +5215,16 @@
         <v>134</v>
       </c>
       <c r="D129" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E129" t="s">
         <v>391</v>
       </c>
       <c r="F129" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G129" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -5244,10 +5244,10 @@
         <v>392</v>
       </c>
       <c r="F130" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G130" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -5267,10 +5267,10 @@
         <v>393</v>
       </c>
       <c r="F131" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G131" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -5290,10 +5290,10 @@
         <v>394</v>
       </c>
       <c r="F132" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G132" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>